<commit_message>
Adjusted elec/BDSBaPCF so that nuclear bids at its expected capacity factor of 92% rather than its peak capacity factor.
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove renewables from BAU guaranteed dispatch and set coal to bid at its expected capacity factor
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A1020E-B0C4-4F04-8009-3AA729898980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="23955" windowHeight="11580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>BDSBaPCF Boolean Do Suppliers Bid at Peak Capacity Factors</t>
   </si>
@@ -128,12 +141,21 @@
   </si>
   <si>
     <t>Do Suppliers Bid at Peak Capacity Factors (Boolean)</t>
+  </si>
+  <si>
+    <t>For the United States, we have set coal to 0 as of version 3.4. This reflects</t>
+  </si>
+  <si>
+    <t>the fact that certain air quality / environmental restrictions, as well as current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supply chain logistics, limit the amount the coal dispatches annually. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,6 +292,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -305,6 +344,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,19 +536,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,84 +558,99 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -586,36 +659,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -623,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -631,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -639,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -647,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -655,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -663,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -671,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -679,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -687,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -695,16 +768,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13">
         <f>B2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -713,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -722,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -731,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>

</xml_diff>